<commit_message>
added 3 2013 events and plots
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
   <si>
     <t>EventName</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Earthquake</t>
-  </si>
-  <si>
-    <t>QZ8501</t>
   </si>
   <si>
     <t>Date</t>
@@ -381,6 +378,30 @@
   </si>
   <si>
     <t>Typhoon Haiyan</t>
+  </si>
+  <si>
+    <t>chelyabinsk, meteor, explosion</t>
+  </si>
+  <si>
+    <t>2013_02_15_07</t>
+  </si>
+  <si>
+    <t>savar, rana, collapse</t>
+  </si>
+  <si>
+    <t>2013_04_24_10</t>
+  </si>
+  <si>
+    <t>2014_04_15_11</t>
+  </si>
+  <si>
+    <t>haiyan, typhoon, philippines</t>
+  </si>
+  <si>
+    <t>2013_11_09_03</t>
+  </si>
+  <si>
+    <t>qz8501</t>
   </si>
 </sst>
 </file>
@@ -427,7 +448,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +469,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -490,11 +517,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -546,55 +590,72 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="15" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="59">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="8" builtinId="46"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -928,16 +989,16 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.75" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.75" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.75" bestFit="1" customWidth="1"/>
@@ -948,13 +1009,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>1</v>
@@ -970,431 +1031,451 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="12">
-        <v>41745</v>
-      </c>
-      <c r="D2" s="16">
-        <v>8.3333333333333329E-2</v>
+      <c r="A2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="11">
+        <v>42087</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.4375</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>40</v>
+        <v>81</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="11">
+        <v>41379</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="12">
-        <v>42119</v>
-      </c>
-      <c r="D3" s="10">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="12">
-        <v>42136</v>
-      </c>
-      <c r="D4" s="16">
-        <v>0.375</v>
+      <c r="C4" s="11">
+        <v>42126</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.22916666666666666</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="11">
+        <v>41320</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="11">
+        <v>41744</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="G6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="11">
+        <v>41765</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="11">
+        <v>42096</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="12">
-        <v>42126</v>
-      </c>
-      <c r="D5" s="10">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="12">
-        <v>41781</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="12">
-        <v>41837</v>
-      </c>
-      <c r="D7" s="16">
-        <v>0.625</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="12">
-        <v>42001</v>
-      </c>
-      <c r="D8" s="16">
-        <v>0.125</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="G8" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="12">
-        <v>42087</v>
-      </c>
-      <c r="D9" s="16">
-        <v>0.4375</v>
-      </c>
+      <c r="A9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="11">
+        <v>41779</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>21</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="17" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="12">
-        <v>41379</v>
-      </c>
-      <c r="D10" s="16">
-        <v>0.79166666666666663</v>
+        <v>94</v>
+      </c>
+      <c r="C10" s="11">
+        <v>41837</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0.625</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="12">
-        <v>41989</v>
+      <c r="A11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="11">
+        <v>42119</v>
       </c>
       <c r="D11" s="10">
         <v>0.29166666666666669</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>35</v>
+      <c r="E11" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>37</v>
+        <v>76</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="15" t="s">
-        <v>44</v>
+      <c r="A12" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="12">
-        <v>42096</v>
-      </c>
-      <c r="D12" s="16">
-        <v>0.16666666666666666</v>
+        <v>92</v>
+      </c>
+      <c r="C12" s="11">
+        <v>42136</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0.375</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>71</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="15" t="s">
-        <v>54</v>
+      <c r="A13" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="12">
-        <v>41744</v>
-      </c>
-      <c r="D13" s="16">
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="C13" s="11">
+        <v>41795</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="11">
+        <v>41989</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="11">
+        <v>42001</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0.125</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="11">
+        <v>41388</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="11">
+        <v>41745</v>
+      </c>
+      <c r="D17" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="11">
+        <v>41781</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="12">
-        <v>41765</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="12">
-        <v>41779</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="12">
-        <v>41795</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="9" t="s">
+      <c r="G18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="12">
-        <v>41320</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="12">
-        <v>41388</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H18" s="9" t="s">
+    <row r="19" spans="1:8">
+      <c r="A19" s="13" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="15" t="s">
+      <c r="B19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="11">
+        <v>41587</v>
+      </c>
+      <c r="D19" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="12">
-        <v>41585</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="8" t="s">
+      <c r="F19" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="14"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1"/>
@@ -1404,7 +1485,7 @@
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="14"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
@@ -1414,7 +1495,7 @@
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="14"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
@@ -1424,7 +1505,7 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="14"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
@@ -1434,7 +1515,7 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="14"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="1"/>
@@ -1444,7 +1525,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="14"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="1"/>
@@ -1454,7 +1535,7 @@
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="14"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
@@ -1464,7 +1545,7 @@
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="14"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
@@ -1474,7 +1555,7 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="14"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
@@ -1484,8 +1565,8 @@
       <c r="H28" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:I28">
-    <sortCondition ref="G1"/>
+  <sortState ref="A2:H28">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1520,10 +1601,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1536,34 +1617,34 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add sydney_hostage and edcow, watis results
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8920" yWindow="1900" windowWidth="30460" windowHeight="19480" tabRatio="500"/>
+    <workbookView xWindow="3000" yWindow="1400" windowWidth="43240" windowHeight="20220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
   <si>
     <t>EventName</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>AirAsia, Aircraft crash</t>
-  </si>
-  <si>
-    <t>4U9525</t>
   </si>
   <si>
     <t>4u9525, gwi18g, germanwings</t>
@@ -245,6 +242,9 @@
     <t>TE4</t>
   </si>
   <si>
+    <t>TE5</t>
+  </si>
+  <si>
     <t>EventTime</t>
   </si>
   <si>
@@ -390,6 +390,44 @@
   </si>
   <si>
     <t>2013_10_11_20</t>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Schriftart für Textkörper"/>
+        <family val="2"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Schriftart für Textkörper"/>
+        <family val="2"/>
+      </rPr>
+      <t>9525</t>
+    </r>
+  </si>
+  <si>
+    <t>sydney_hostage</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>sydney, hostage</t>
+  </si>
+  <si>
+    <t>Terrorist attack on Café in Sydney</t>
+  </si>
+  <si>
+    <t>2014_12_15_02</t>
   </si>
 </sst>
 </file>
@@ -499,11 +537,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="88">
+  <cellStyleXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -608,7 +674,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="88">
+  <cellStyles count="116">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -653,6 +719,20 @@
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -695,6 +775,20 @@
     <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1025,10 +1119,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1070,8 +1165,8 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="12" t="s">
-        <v>19</v>
+      <c r="A2" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>74</v>
@@ -1083,21 +1178,21 @@
         <v>0.4375</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>69</v>
@@ -1109,21 +1204,21 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>71</v>
@@ -1135,16 +1230,16 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1175,7 +1270,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>94</v>
@@ -1187,21 +1282,21 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>76</v>
@@ -1213,16 +1308,16 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1239,13 +1334,13 @@
         <v>0.625</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>17</v>
@@ -1253,7 +1348,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>77</v>
@@ -1271,7 +1366,7 @@
         <v>14</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>10</v>
@@ -1279,7 +1374,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>70</v>
@@ -1294,18 +1389,18 @@
         <v>3</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>75</v>
@@ -1317,16 +1412,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1343,13 +1438,13 @@
         <v>0.125</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>18</v>
@@ -1486,14 +1581,30 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="12"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
+      <c r="A18" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="11">
+        <v>41988</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="12"/>
@@ -1541,6 +1652,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -1562,10 +1674,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1586,26 +1698,26 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>